<commit_message>
Masked the actual names
</commit_message>
<xml_diff>
--- a/files/students_participation_tracker_BP.xlsx
+++ b/files/students_participation_tracker_BP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://niuits-my.sharepoint.com/personal/z2007047_students_niu_edu/Documents/Desktop/Vineel/Vineel/TA work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://niuits-my.sharepoint.com/personal/z2007047_students_niu_edu/Documents/Desktop/Vineel/Vineel/TA work/Quarto Project/omis_dashboard/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="8_{1C248454-4DBB-D844-9FFD-1D80DC44F931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9821A96-019D-46A4-A398-4062E8391465}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="8_{1C248454-4DBB-D844-9FFD-1D80DC44F931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47C6C272-3084-4620-A4ED-7768B8FC95DD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A567C43-350C-4CC6-BB4B-171D59AA692F}"/>
   </bookViews>
@@ -43,81 +43,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Arens, Ryan Peter</t>
-  </si>
-  <si>
-    <t>Bertrand, Monica</t>
-  </si>
-  <si>
-    <t>Estrada Jr, Camilo</t>
-  </si>
-  <si>
-    <t>Fitch, Jordan</t>
-  </si>
-  <si>
-    <t>Frew, RJ Thomas</t>
-  </si>
-  <si>
-    <t>Ikpidungise, Ubonobong</t>
-  </si>
-  <si>
-    <t>Johnson, Jacob Mitchell</t>
-  </si>
-  <si>
-    <t>Koschtojan, Armin</t>
-  </si>
-  <si>
-    <t>Linkletter, Ryan</t>
-  </si>
-  <si>
-    <t>Loth, Brandon</t>
-  </si>
-  <si>
-    <t>Mejia Garcia, Francisco Daniel</t>
-  </si>
-  <si>
-    <t>Mendez, Yary Lizbeth</t>
-  </si>
-  <si>
-    <t>Murtaza, Mizo Muzzammil</t>
-  </si>
-  <si>
-    <t>Newman, Alex Jacob</t>
-  </si>
-  <si>
-    <t>Olson, Erik</t>
-  </si>
-  <si>
-    <t>Predki, Jason Mitchell</t>
-  </si>
-  <si>
-    <t>Ramirez, Ines Liana</t>
-  </si>
-  <si>
-    <t>Rodriguez, Manuel Alvaro</t>
-  </si>
-  <si>
-    <t>Shah, Aalap</t>
-  </si>
-  <si>
-    <t>Swadhin, Nirovro Niloy</t>
-  </si>
-  <si>
-    <t>Syed, Zahra Fatima</t>
-  </si>
-  <si>
-    <t>Vazquez, Jacob Alejandro</t>
-  </si>
-  <si>
-    <t>Weiland, Skylar Andrew</t>
-  </si>
-  <si>
-    <t>Wilson, Joseph</t>
-  </si>
-  <si>
-    <t>Zirk, Lydia</t>
-  </si>
-  <si>
     <t>Bandlamudi, Saiteja</t>
   </si>
   <si>
@@ -302,6 +227,81 @@
   </si>
   <si>
     <t>teams_score</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -427,14 +427,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -472,7 +468,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -578,7 +574,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -720,7 +716,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -732,7 +728,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E11" sqref="E11"/>
+      <selection pane="topRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,33 +749,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1">
         <v>12</v>
@@ -803,7 +799,7 @@
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1">
         <v>8</v>
@@ -829,7 +825,7 @@
     </row>
     <row r="4" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -857,7 +853,7 @@
     </row>
     <row r="5" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1">
         <v>13</v>
@@ -883,7 +879,7 @@
     </row>
     <row r="6" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -907,7 +903,7 @@
     </row>
     <row r="7" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>
@@ -931,7 +927,7 @@
     </row>
     <row r="8" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -959,7 +955,7 @@
     </row>
     <row r="9" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1">
         <v>23</v>
@@ -989,7 +985,7 @@
     </row>
     <row r="10" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="B10" s="1">
         <v>4</v>
@@ -1015,7 +1011,7 @@
     </row>
     <row r="11" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1">
@@ -1041,7 +1037,7 @@
     </row>
     <row r="12" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1">
         <v>7</v>
@@ -1067,7 +1063,7 @@
     </row>
     <row r="13" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -1093,7 +1089,7 @@
     </row>
     <row r="14" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1117,7 +1113,7 @@
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="B15" s="1">
         <v>47</v>
@@ -1145,7 +1141,7 @@
     </row>
     <row r="16" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1167,7 +1163,7 @@
     </row>
     <row r="17" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -1191,7 +1187,7 @@
     </row>
     <row r="18" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="B18" s="1">
         <v>4</v>
@@ -1221,7 +1217,7 @@
     </row>
     <row r="19" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="B19" s="1">
         <v>9</v>
@@ -1247,7 +1243,7 @@
     </row>
     <row r="20" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B20" s="1">
         <v>8</v>
@@ -1271,7 +1267,7 @@
     </row>
     <row r="21" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -1295,7 +1291,7 @@
     </row>
     <row r="22" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -1323,7 +1319,7 @@
     </row>
     <row r="23" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1347,7 +1343,7 @@
     </row>
     <row r="24" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="B24" s="1">
         <v>24</v>
@@ -1373,7 +1369,7 @@
     </row>
     <row r="25" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="B25" s="1">
         <v>23</v>
@@ -1401,7 +1397,7 @@
     </row>
     <row r="26" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1459,33 +1455,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1507,7 +1503,7 @@
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1529,7 +1525,7 @@
     </row>
     <row r="4" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -1557,7 +1553,7 @@
     </row>
     <row r="5" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1581,7 +1577,7 @@
     </row>
     <row r="6" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1">
@@ -1605,7 +1601,7 @@
     </row>
     <row r="7" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1629,7 +1625,7 @@
     </row>
     <row r="8" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>11</v>
@@ -1655,7 +1651,7 @@
     </row>
     <row r="9" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>6</v>
@@ -1681,7 +1677,7 @@
     </row>
     <row r="10" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
@@ -1711,7 +1707,7 @@
     </row>
     <row r="11" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -1737,7 +1733,7 @@
     </row>
     <row r="12" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>5</v>
@@ -1763,7 +1759,7 @@
     </row>
     <row r="13" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>3</v>
@@ -1791,7 +1787,7 @@
     </row>
     <row r="14" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1815,7 +1811,7 @@
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
@@ -1841,7 +1837,7 @@
     </row>
     <row r="16" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>14</v>
@@ -1869,7 +1865,7 @@
     </row>
     <row r="17" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -1895,7 +1891,7 @@
     </row>
     <row r="18" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>8</v>
@@ -1923,7 +1919,7 @@
     </row>
     <row r="19" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
@@ -1951,7 +1947,7 @@
     </row>
     <row r="20" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1975,7 +1971,7 @@
     </row>
     <row r="21" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -2003,7 +1999,7 @@
     </row>
     <row r="22" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -2029,7 +2025,7 @@
     </row>
     <row r="23" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>4</v>
@@ -2053,7 +2049,7 @@
     </row>
     <row r="24" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>5</v>
@@ -2079,7 +2075,7 @@
     </row>
     <row r="25" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
@@ -2105,7 +2101,7 @@
     </row>
     <row r="26" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>10</v>
@@ -2131,7 +2127,7 @@
     </row>
     <row r="27" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>5</v>
@@ -2159,7 +2155,7 @@
     </row>
     <row r="28" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2183,7 +2179,7 @@
     </row>
     <row r="29" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>2</v>
@@ -2211,7 +2207,7 @@
     </row>
     <row r="30" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>2</v>
@@ -2235,7 +2231,7 @@
     </row>
     <row r="31" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>18</v>
@@ -2267,7 +2263,7 @@
     </row>
     <row r="32" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>10</v>
@@ -2325,33 +2321,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
@@ -2377,7 +2373,7 @@
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1">
         <v>8</v>
@@ -2405,7 +2401,7 @@
     </row>
     <row r="4" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1">
         <v>5</v>
@@ -2433,7 +2429,7 @@
     </row>
     <row r="5" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2455,7 +2451,7 @@
     </row>
     <row r="6" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1">
         <v>10</v>
@@ -2481,7 +2477,7 @@
     </row>
     <row r="7" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1">
         <v>19</v>
@@ -2509,7 +2505,7 @@
     </row>
     <row r="8" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2531,7 +2527,7 @@
     </row>
     <row r="9" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -2559,7 +2555,7 @@
     </row>
     <row r="10" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1">
         <v>11</v>
@@ -2583,7 +2579,7 @@
     </row>
     <row r="11" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -2607,7 +2603,7 @@
     </row>
     <row r="12" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -2635,7 +2631,7 @@
     </row>
     <row r="13" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
@@ -2659,7 +2655,7 @@
     </row>
     <row r="14" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2683,7 +2679,7 @@
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
@@ -2711,7 +2707,7 @@
     </row>
     <row r="16" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -2739,7 +2735,7 @@
     </row>
     <row r="17" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
@@ -2763,7 +2759,7 @@
     </row>
     <row r="18" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1">
         <v>5</v>
@@ -2791,7 +2787,7 @@
     </row>
     <row r="19" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2813,7 +2809,7 @@
     </row>
     <row r="20" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2835,7 +2831,7 @@
     </row>
     <row r="21" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
@@ -2861,7 +2857,7 @@
     </row>
     <row r="22" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2885,7 +2881,7 @@
     </row>
     <row r="23" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
@@ -2911,7 +2907,7 @@
     </row>
     <row r="24" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="B24" s="1">
         <v>2</v>

</xml_diff>